<commit_message>
#update file template excel
</commit_message>
<xml_diff>
--- a/ME-API/Resources/Template/Sixs_Score_Record_Template.xlsx
+++ b/ME-API/Resources/Template/Sixs_Score_Record_Template.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$M$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$L$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Audit_Date</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Rating1</t>
   </si>
   <si>
-    <t>Rating2</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
   </si>
   <si>
     <t>&amp;=result.Rating1</t>
-  </si>
-  <si>
-    <t>&amp;=result.Rating2</t>
   </si>
   <si>
     <t>&amp;=result.Total</t>
@@ -94,8 +88,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -134,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -181,18 +176,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -200,6 +205,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -482,11 +493,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,32 +509,30 @@
     <col min="5" max="5" width="23.140625" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
     <col min="7" max="7" width="24" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.5703125" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,52 +563,46 @@
       <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-    </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="K3" s="4"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>